<commit_message>
sm nm 2023 v 20230611
</commit_message>
<xml_diff>
--- a/mallar/import/sm_nm 2023/extraktion_01-SMNM2023 - med NM.xlsx
+++ b/mallar/import/sm_nm 2023/extraktion_01-SMNM2023 - med NM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\mallar\import\sm_nm 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57500B88-23F2-4DF9-BD1D-60FEF129D5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE99F41-2BEA-48EF-BE71-2EB74F8A8970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" tabRatio="483" xr2:uid="{9C6C5895-3CBC-495A-8EC3-24DF642F0EB2}"/>
+    <workbookView xWindow="43080" yWindow="5310" windowWidth="38640" windowHeight="21240" tabRatio="483" xr2:uid="{9C6C5895-3CBC-495A-8EC3-24DF642F0EB2}"/>
   </bookViews>
   <sheets>
     <sheet name="ekipage" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="362">
   <si>
     <t>Linda Jenvall</t>
   </si>
@@ -1066,9 +1066,6 @@
     <t>Olga Fagerström</t>
   </si>
   <si>
-    <t>Startordning på Halving?</t>
-  </si>
-  <si>
     <t>Danmark</t>
   </si>
   <si>
@@ -1103,6 +1100,30 @@
   </si>
   <si>
     <t>Team Cassiopeia</t>
+  </si>
+  <si>
+    <t>Genevieve Dowen</t>
+  </si>
+  <si>
+    <t>Arnika Palomurto</t>
+  </si>
+  <si>
+    <t>Startordning på Kaliostro?</t>
+  </si>
+  <si>
+    <t>Neea Kostiainen, Kerttu Saarimaa, Matilda Sjöström, Vilma Granberg</t>
+  </si>
+  <si>
+    <t>Kerttu Saarimaa</t>
+  </si>
+  <si>
+    <t>Matilda Sjöström</t>
+  </si>
+  <si>
+    <t>Vilma Granberg</t>
+  </si>
+  <si>
+    <t>Linnea, Amalia Glimmerhav, Edla Danielsson, Anna-Liisa Anson</t>
   </si>
 </sst>
 </file>
@@ -1493,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B3B0E3-2027-4083-B582-AAB0C4C3F786}">
-  <dimension ref="A1:W108"/>
+  <dimension ref="A1:W114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1689,7 +1710,7 @@
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="L3">
         <v>115495</v>
@@ -2380,13 +2401,13 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>629742</v>
+        <v>629745</v>
       </c>
       <c r="B17" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D17">
         <v>95073</v>
@@ -2401,42 +2422,39 @@
         <v>116</v>
       </c>
       <c r="H17">
-        <v>609</v>
+        <v>1330</v>
       </c>
       <c r="I17" t="s">
-        <v>29</v>
-      </c>
-      <c r="J17" t="s">
-        <v>181</v>
+        <v>55</v>
       </c>
       <c r="L17">
-        <v>60750</v>
+        <v>119967</v>
       </c>
       <c r="M17" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>629745</v>
+        <v>629742</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C18" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D18">
-        <v>69289</v>
+        <v>95073</v>
       </c>
       <c r="E18" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F18">
-        <v>301468</v>
+        <v>279357</v>
       </c>
       <c r="G18" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H18">
         <v>609</v>
@@ -2444,11 +2462,14 @@
       <c r="I18" t="s">
         <v>29</v>
       </c>
+      <c r="J18" t="s">
+        <v>181</v>
+      </c>
       <c r="L18">
-        <v>131893</v>
+        <v>60750</v>
       </c>
       <c r="M18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.45">
@@ -2462,28 +2483,28 @@
         <v>153</v>
       </c>
       <c r="D19">
-        <v>40552</v>
+        <v>69289</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>127</v>
       </c>
       <c r="F19">
-        <v>293760</v>
+        <v>301468</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>114</v>
       </c>
       <c r="H19">
-        <v>223</v>
+        <v>609</v>
       </c>
       <c r="I19" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="L19">
-        <v>69830</v>
+        <v>131893</v>
       </c>
       <c r="M19" t="s">
-        <v>24</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.45">
@@ -2509,16 +2530,16 @@
         <v>14</v>
       </c>
       <c r="H20">
-        <v>869</v>
+        <v>223</v>
       </c>
       <c r="I20" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="L20">
-        <v>120827</v>
+        <v>69830</v>
       </c>
       <c r="M20" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.45">
@@ -2532,31 +2553,28 @@
         <v>153</v>
       </c>
       <c r="D21">
-        <v>39883</v>
+        <v>40552</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="F21">
-        <v>310234</v>
+        <v>293760</v>
       </c>
       <c r="G21" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="H21">
-        <v>1198</v>
+        <v>869</v>
       </c>
       <c r="I21" t="s">
-        <v>48</v>
-      </c>
-      <c r="J21" t="s">
-        <v>182</v>
+        <v>12</v>
       </c>
       <c r="L21">
-        <v>134138</v>
+        <v>120827</v>
       </c>
       <c r="M21" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.45">
@@ -2570,31 +2588,31 @@
         <v>153</v>
       </c>
       <c r="D22">
-        <v>40552</v>
+        <v>39883</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="F22">
-        <v>293760</v>
+        <v>310234</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="H22">
-        <v>223</v>
+        <v>1198</v>
       </c>
       <c r="I22" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="J22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L22">
-        <v>134608</v>
+        <v>134138</v>
       </c>
       <c r="M22" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.45">
@@ -2608,28 +2626,31 @@
         <v>153</v>
       </c>
       <c r="D23">
-        <v>39883</v>
+        <v>40552</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="F23">
-        <v>310234</v>
+        <v>293760</v>
       </c>
       <c r="G23" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="H23">
-        <v>1198</v>
+        <v>223</v>
       </c>
       <c r="I23" t="s">
-        <v>48</v>
+        <v>2</v>
+      </c>
+      <c r="J23" t="s">
+        <v>183</v>
       </c>
       <c r="L23">
-        <v>107961</v>
+        <v>134608</v>
       </c>
       <c r="M23" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.45">
@@ -2643,31 +2664,28 @@
         <v>153</v>
       </c>
       <c r="D24">
-        <v>65038</v>
+        <v>39883</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F24">
-        <v>312598</v>
+        <v>310234</v>
       </c>
       <c r="G24" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H24">
-        <v>223</v>
+        <v>1198</v>
       </c>
       <c r="I24" t="s">
-        <v>2</v>
-      </c>
-      <c r="J24" t="s">
-        <v>184</v>
+        <v>48</v>
       </c>
       <c r="L24">
-        <v>101580</v>
+        <v>107961</v>
       </c>
       <c r="M24" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.45">
@@ -2681,16 +2699,16 @@
         <v>153</v>
       </c>
       <c r="D25">
-        <v>36847</v>
+        <v>65038</v>
       </c>
       <c r="E25" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="F25">
-        <v>280330</v>
+        <v>312598</v>
       </c>
       <c r="G25" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="H25">
         <v>223</v>
@@ -2699,13 +2717,13 @@
         <v>2</v>
       </c>
       <c r="J25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L25">
-        <v>101407</v>
+        <v>101580</v>
       </c>
       <c r="M25" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.45">
@@ -2719,28 +2737,31 @@
         <v>153</v>
       </c>
       <c r="D26">
-        <v>39883</v>
+        <v>36847</v>
       </c>
       <c r="E26" t="s">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>310234</v>
+        <v>280330</v>
       </c>
       <c r="G26" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="H26">
-        <v>1198</v>
+        <v>223</v>
       </c>
       <c r="I26" t="s">
-        <v>48</v>
+        <v>2</v>
+      </c>
+      <c r="J26" t="s">
+        <v>185</v>
       </c>
       <c r="L26">
-        <v>108087</v>
+        <v>101407</v>
       </c>
       <c r="M26" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.45">
@@ -2754,31 +2775,28 @@
         <v>153</v>
       </c>
       <c r="D27">
-        <v>36847</v>
+        <v>39883</v>
       </c>
       <c r="E27" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="F27">
-        <v>264133</v>
+        <v>310234</v>
       </c>
       <c r="G27" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="H27">
-        <v>223</v>
+        <v>1198</v>
       </c>
       <c r="I27" t="s">
-        <v>2</v>
-      </c>
-      <c r="J27" t="s">
-        <v>186</v>
+        <v>48</v>
       </c>
       <c r="L27">
-        <v>109403</v>
+        <v>108087</v>
       </c>
       <c r="M27" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.45">
@@ -2810,13 +2828,13 @@
         <v>2</v>
       </c>
       <c r="J28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L28">
-        <v>150025</v>
+        <v>109403</v>
       </c>
       <c r="M28" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.45">
@@ -2830,28 +2848,31 @@
         <v>153</v>
       </c>
       <c r="D29">
-        <v>95073</v>
+        <v>36847</v>
       </c>
       <c r="E29" t="s">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>279357</v>
+        <v>264133</v>
       </c>
       <c r="G29" t="s">
-        <v>116</v>
+        <v>1</v>
       </c>
       <c r="H29">
-        <v>1330</v>
+        <v>223</v>
       </c>
       <c r="I29" t="s">
-        <v>55</v>
+        <v>2</v>
+      </c>
+      <c r="J29" t="s">
+        <v>187</v>
       </c>
       <c r="L29">
-        <v>119967</v>
+        <v>150025</v>
       </c>
       <c r="M29" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.45">
@@ -4122,170 +4143,170 @@
         <v>277</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A64">
-        <v>629741</v>
-      </c>
-      <c r="B64">
-        <v>24</v>
-      </c>
-      <c r="C64" t="s">
-        <v>147</v>
-      </c>
-      <c r="D64">
-        <v>188520</v>
-      </c>
-      <c r="E64" t="s">
-        <v>128</v>
-      </c>
-      <c r="F64">
-        <v>313507</v>
-      </c>
-      <c r="G64" t="s">
-        <v>115</v>
-      </c>
-      <c r="H64">
-        <v>202</v>
-      </c>
-      <c r="I64" t="s">
-        <v>261</v>
-      </c>
-      <c r="J64" t="s">
-        <v>321</v>
-      </c>
-      <c r="L64">
-        <v>1007</v>
-      </c>
-      <c r="M64" t="s">
-        <v>278</v>
+    <row r="64" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="7">
+        <v>629756</v>
+      </c>
+      <c r="B64" s="7">
+        <v>15</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D64" s="7">
+        <v>101</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="F64" s="7">
+        <v>2</v>
+      </c>
+      <c r="G64" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H64" s="7">
+        <v>210</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="L64" s="7">
+        <v>1053</v>
+      </c>
+      <c r="M64" s="7" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A65">
-        <v>629747</v>
+        <v>629741</v>
       </c>
       <c r="B65">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C65" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D65">
-        <v>104</v>
+        <v>188520</v>
       </c>
       <c r="E65" t="s">
-        <v>251</v>
+        <v>128</v>
       </c>
       <c r="F65">
-        <v>3</v>
+        <v>313507</v>
       </c>
       <c r="G65" t="s">
-        <v>229</v>
+        <v>115</v>
       </c>
       <c r="H65">
-        <v>201</v>
-      </c>
-      <c r="I65" s="2" t="s">
-        <v>260</v>
+        <v>202</v>
+      </c>
+      <c r="I65" t="s">
+        <v>261</v>
+      </c>
+      <c r="J65" t="s">
+        <v>321</v>
       </c>
       <c r="L65">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="M65" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A66">
-        <v>629756</v>
+        <v>629747</v>
       </c>
       <c r="B66">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C66" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D66">
-        <v>188520</v>
+        <v>104</v>
       </c>
       <c r="E66" t="s">
-        <v>128</v>
+        <v>251</v>
       </c>
       <c r="F66">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G66" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H66">
-        <v>210</v>
-      </c>
-      <c r="I66" t="s">
-        <v>322</v>
+        <v>201</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>260</v>
       </c>
       <c r="L66">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="M66" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A67">
-        <v>629738</v>
+        <v>629756</v>
       </c>
       <c r="B67">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C67" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="D67">
-        <v>105</v>
+        <v>188520</v>
       </c>
       <c r="E67" t="s">
-        <v>252</v>
+        <v>128</v>
       </c>
       <c r="F67">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G67" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H67">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="I67" t="s">
-        <v>258</v>
+        <v>322</v>
       </c>
       <c r="L67">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="M67" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A68">
-        <v>629744</v>
+        <v>629738</v>
       </c>
       <c r="B68">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C68" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D68">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E68" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F68">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G68" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H68">
         <v>200</v>
@@ -4293,14 +4314,11 @@
       <c r="I68" t="s">
         <v>258</v>
       </c>
-      <c r="J68" t="s">
-        <v>324</v>
-      </c>
       <c r="L68">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="M68" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.45">
@@ -4331,22 +4349,25 @@
       <c r="I69" t="s">
         <v>258</v>
       </c>
+      <c r="J69" t="s">
+        <v>324</v>
+      </c>
       <c r="L69">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="M69" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A70">
-        <v>629747</v>
+        <v>629744</v>
       </c>
       <c r="B70">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C70" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D70">
         <v>106</v>
@@ -4367,48 +4388,45 @@
         <v>258</v>
       </c>
       <c r="L70">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="M70" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A71">
-        <v>629744</v>
+        <v>629747</v>
       </c>
       <c r="B71">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C71" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D71">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E71" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F71">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G71" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H71">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I71" t="s">
-        <v>262</v>
-      </c>
-      <c r="J71" t="s">
-        <v>325</v>
+        <v>258</v>
       </c>
       <c r="L71">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="M71" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.45">
@@ -4439,22 +4457,25 @@
       <c r="I72" t="s">
         <v>262</v>
       </c>
+      <c r="J72" t="s">
+        <v>325</v>
+      </c>
       <c r="L72">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="M72" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A73">
-        <v>629741</v>
+        <v>629744</v>
       </c>
       <c r="B73">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C73" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D73">
         <v>107</v>
@@ -4463,10 +4484,10 @@
         <v>254</v>
       </c>
       <c r="F73">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G73" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H73">
         <v>203</v>
@@ -4474,60 +4495,60 @@
       <c r="I73" t="s">
         <v>262</v>
       </c>
-      <c r="J73" t="s">
-        <v>326</v>
-      </c>
       <c r="L73">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="M73" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A74">
-        <v>629744</v>
-      </c>
-      <c r="B74">
-        <v>25</v>
-      </c>
-      <c r="C74" t="s">
-        <v>151</v>
-      </c>
-      <c r="D74">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A74" s="8">
+        <v>629754</v>
+      </c>
+      <c r="B74" s="8">
+        <v>13</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D74" s="7">
         <v>107</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="F74">
-        <v>10</v>
-      </c>
-      <c r="G74" t="s">
-        <v>236</v>
-      </c>
-      <c r="H74">
+      <c r="F74" s="7">
+        <v>9</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="H74" s="7">
         <v>203</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I74" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="L74">
-        <v>1017</v>
-      </c>
-      <c r="M74" t="s">
-        <v>288</v>
+      <c r="J74" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="L74" s="7">
+        <v>1054</v>
+      </c>
+      <c r="M74" s="7" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A75">
-        <v>629747</v>
+        <v>629741</v>
       </c>
       <c r="B75">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C75" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D75">
         <v>107</v>
@@ -4548,24 +4569,24 @@
         <v>262</v>
       </c>
       <c r="J75" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L75">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="M75" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A76">
-        <v>629747</v>
+        <v>629744</v>
       </c>
       <c r="B76">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C76" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D76">
         <v>107</v>
@@ -4586,21 +4607,21 @@
         <v>262</v>
       </c>
       <c r="L76">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="M76" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A77">
-        <v>629738</v>
+        <v>629747</v>
       </c>
       <c r="B77">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C77" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="D77">
         <v>107</v>
@@ -4609,36 +4630,36 @@
         <v>254</v>
       </c>
       <c r="F77">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G77" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H77">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I77" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J77" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L77">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="M77" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A78">
-        <v>629744</v>
+        <v>629747</v>
       </c>
       <c r="B78">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C78" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D78">
         <v>107</v>
@@ -4647,33 +4668,33 @@
         <v>254</v>
       </c>
       <c r="F78">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G78" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H78">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I78" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L78">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="M78" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A79">
-        <v>629744</v>
+        <v>629738</v>
       </c>
       <c r="B79">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C79" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D79">
         <v>107</v>
@@ -4694,13 +4715,13 @@
         <v>264</v>
       </c>
       <c r="J79" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L79">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="M79" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.45">
@@ -4732,48 +4753,48 @@
         <v>264</v>
       </c>
       <c r="L80">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="M80" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A81">
-        <v>629747</v>
+        <v>629744</v>
       </c>
       <c r="B81">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C81" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D81">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E81" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F81">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G81" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H81">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I81" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J81" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L81">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="M81" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.45">
@@ -4787,39 +4808,39 @@
         <v>151</v>
       </c>
       <c r="D82">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E82" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F82">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G82" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H82">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I82" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L82">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="M82" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A83">
-        <v>629758</v>
+        <v>629747</v>
       </c>
       <c r="B83">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C83" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D83">
         <v>109</v>
@@ -4839,22 +4860,25 @@
       <c r="I83" t="s">
         <v>265</v>
       </c>
+      <c r="J83" t="s">
+        <v>330</v>
+      </c>
       <c r="L83">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="M83" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A84">
-        <v>629747</v>
+        <v>629744</v>
       </c>
       <c r="B84">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C84" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D84">
         <v>109</v>
@@ -4875,94 +4899,91 @@
         <v>265</v>
       </c>
       <c r="L84">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="M84" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A85">
-        <v>629747</v>
+        <v>629758</v>
       </c>
       <c r="B85">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C85" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="D85">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E85" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F85">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G85" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H85">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I85" t="s">
-        <v>266</v>
-      </c>
-      <c r="J85" t="s">
-        <v>331</v>
+        <v>265</v>
       </c>
       <c r="L85">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="M85" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="86" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A86">
-        <v>629744</v>
+        <v>629747</v>
       </c>
       <c r="B86">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C86" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D86">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E86" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F86">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G86" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H86">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I86" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="L86">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="M86" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="87" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A87">
-        <v>629756</v>
+        <v>629747</v>
       </c>
       <c r="B87">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C87" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D87">
         <v>110</v>
@@ -4982,22 +5003,25 @@
       <c r="I87" t="s">
         <v>266</v>
       </c>
+      <c r="J87" t="s">
+        <v>331</v>
+      </c>
       <c r="L87">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="M87" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A88">
-        <v>630356</v>
+        <v>629744</v>
       </c>
       <c r="B88">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C88" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="D88">
         <v>110</v>
@@ -5017,107 +5041,104 @@
       <c r="I88" t="s">
         <v>266</v>
       </c>
-      <c r="J88" t="s">
-        <v>302</v>
-      </c>
-      <c r="K88" t="s">
-        <v>332</v>
-      </c>
       <c r="L88">
         <v>1029</v>
       </c>
       <c r="M88" t="s">
         <v>300</v>
       </c>
-      <c r="N88">
-        <v>1028</v>
-      </c>
-      <c r="O88" t="s">
-        <v>299</v>
-      </c>
     </row>
     <row r="89" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A89">
-        <v>629744</v>
+        <v>629756</v>
       </c>
       <c r="B89">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C89" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="D89">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E89" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="F89">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G89" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H89">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="I89" t="s">
-        <v>262</v>
-      </c>
-      <c r="J89" t="s">
-        <v>333</v>
+        <v>266</v>
       </c>
       <c r="L89">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="M89" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="90" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A90">
-        <v>629744</v>
+        <v>630356</v>
       </c>
       <c r="B90">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C90" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="D90">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E90" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="F90">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G90" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H90">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="I90" t="s">
-        <v>262</v>
+        <v>266</v>
+      </c>
+      <c r="J90" t="s">
+        <v>302</v>
+      </c>
+      <c r="K90" t="s">
+        <v>332</v>
       </c>
       <c r="L90">
-        <v>1033</v>
+        <v>1029</v>
       </c>
       <c r="M90" t="s">
-        <v>304</v>
+        <v>300</v>
+      </c>
+      <c r="N90">
+        <v>1028</v>
+      </c>
+      <c r="O90" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="91" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A91">
-        <v>629747</v>
+        <v>629744</v>
       </c>
       <c r="B91">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C91" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D91">
         <v>100</v>
@@ -5137,49 +5158,49 @@
       <c r="I91" t="s">
         <v>262</v>
       </c>
+      <c r="J91" t="s">
+        <v>333</v>
+      </c>
       <c r="L91">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="M91" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="92" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A92">
-        <v>629747</v>
+        <v>629744</v>
       </c>
       <c r="B92">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C92" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D92">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E92" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="F92">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G92" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H92">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I92" t="s">
-        <v>267</v>
-      </c>
-      <c r="J92" t="s">
-        <v>334</v>
+        <v>262</v>
       </c>
       <c r="L92">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="M92" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="93" spans="1:23" x14ac:dyDescent="0.45">
@@ -5193,148 +5214,112 @@
         <v>155</v>
       </c>
       <c r="D93">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E93" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="F93">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G93" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H93">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I93" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="L93">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="M93" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A94">
-        <v>629732</v>
+        <v>629747</v>
       </c>
       <c r="B94">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C94" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="D94">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E94" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="F94">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G94" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H94">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I94" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J94" t="s">
-        <v>335</v>
-      </c>
-      <c r="K94" t="s">
-        <v>308</v>
+        <v>334</v>
       </c>
       <c r="L94">
-        <v>1049</v>
+        <v>1035</v>
       </c>
       <c r="M94" t="s">
-        <v>336</v>
-      </c>
-      <c r="N94">
-        <v>1039</v>
-      </c>
-      <c r="O94" t="s">
-        <v>310</v>
-      </c>
-      <c r="P94">
-        <v>1050</v>
-      </c>
-      <c r="Q94" t="s">
-        <v>337</v>
-      </c>
-      <c r="R94">
-        <v>1040</v>
-      </c>
-      <c r="S94" t="s">
-        <v>311</v>
-      </c>
-      <c r="T94">
-        <v>1018</v>
-      </c>
-      <c r="U94" t="s">
-        <v>289</v>
-      </c>
-      <c r="V94">
-        <v>1038</v>
-      </c>
-      <c r="W94" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="95" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A95">
-        <v>629738</v>
+        <v>629747</v>
       </c>
       <c r="B95">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C95" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="D95">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E95" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="F95">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G95" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H95">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I95" t="s">
-        <v>268</v>
-      </c>
-      <c r="J95" t="s">
-        <v>338</v>
+        <v>267</v>
       </c>
       <c r="L95">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="M95" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="96" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A96">
-        <v>629744</v>
+        <v>629732</v>
       </c>
       <c r="B96">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C96" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="D96">
         <v>102</v>
@@ -5343,10 +5328,10 @@
         <v>249</v>
       </c>
       <c r="F96">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G96" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H96">
         <v>208</v>
@@ -5354,22 +5339,58 @@
       <c r="I96" t="s">
         <v>268</v>
       </c>
+      <c r="J96" t="s">
+        <v>335</v>
+      </c>
+      <c r="K96" t="s">
+        <v>308</v>
+      </c>
       <c r="L96">
+        <v>1049</v>
+      </c>
+      <c r="M96" t="s">
+        <v>336</v>
+      </c>
+      <c r="N96">
         <v>1039</v>
       </c>
-      <c r="M96" t="s">
+      <c r="O96" t="s">
         <v>310</v>
+      </c>
+      <c r="P96">
+        <v>1050</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>337</v>
+      </c>
+      <c r="R96">
+        <v>1040</v>
+      </c>
+      <c r="S96" t="s">
+        <v>311</v>
+      </c>
+      <c r="T96">
+        <v>1018</v>
+      </c>
+      <c r="U96" t="s">
+        <v>289</v>
+      </c>
+      <c r="V96">
+        <v>1038</v>
+      </c>
+      <c r="W96" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="97" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A97">
-        <v>629747</v>
+        <v>629738</v>
       </c>
       <c r="B97">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C97" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D97">
         <v>102</v>
@@ -5378,10 +5399,10 @@
         <v>249</v>
       </c>
       <c r="F97">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G97" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H97">
         <v>208</v>
@@ -5389,22 +5410,25 @@
       <c r="I97" t="s">
         <v>268</v>
       </c>
+      <c r="J97" t="s">
+        <v>338</v>
+      </c>
       <c r="L97">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="M97" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="98" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A98">
-        <v>629747</v>
+        <v>629744</v>
       </c>
       <c r="B98">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C98" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D98">
         <v>102</v>
@@ -5413,10 +5437,10 @@
         <v>249</v>
       </c>
       <c r="F98">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G98" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H98">
         <v>208</v>
@@ -5424,14 +5448,11 @@
       <c r="I98" t="s">
         <v>268</v>
       </c>
-      <c r="J98" t="s">
-        <v>339</v>
-      </c>
       <c r="L98">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="M98" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="99" spans="1:23" x14ac:dyDescent="0.45">
@@ -5451,10 +5472,10 @@
         <v>249</v>
       </c>
       <c r="F99">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G99" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H99">
         <v>208</v>
@@ -5462,152 +5483,119 @@
       <c r="I99" t="s">
         <v>268</v>
       </c>
+      <c r="J99" s="3" t="s">
+        <v>357</v>
+      </c>
       <c r="L99">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="M99" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A100">
-        <v>629747</v>
-      </c>
-      <c r="B100">
-        <v>26</v>
-      </c>
-      <c r="C100" t="s">
-        <v>155</v>
-      </c>
-      <c r="D100">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A100" s="7">
+        <v>629759</v>
+      </c>
+      <c r="B100" s="7">
+        <v>18</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="D100" s="7">
         <v>102</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E100" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="F100">
-        <v>19</v>
-      </c>
-      <c r="G100" t="s">
-        <v>245</v>
-      </c>
-      <c r="H100">
+      <c r="F100" s="7">
+        <v>18</v>
+      </c>
+      <c r="G100" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="H100" s="7">
         <v>208</v>
       </c>
-      <c r="I100" t="s">
+      <c r="I100" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="L100">
-        <v>1043</v>
-      </c>
-      <c r="M100" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A101">
-        <v>629747</v>
-      </c>
-      <c r="B101">
-        <v>26</v>
-      </c>
-      <c r="C101" t="s">
-        <v>155</v>
-      </c>
-      <c r="D101">
+      <c r="L100" s="7">
+        <v>1055</v>
+      </c>
+      <c r="M100" s="7" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A101" s="7">
+        <v>629759</v>
+      </c>
+      <c r="B101" s="7">
+        <v>18</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="D101" s="7">
         <v>102</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="F101">
-        <v>19</v>
-      </c>
-      <c r="G101" t="s">
-        <v>245</v>
-      </c>
-      <c r="H101">
+      <c r="F101" s="7">
+        <v>18</v>
+      </c>
+      <c r="G101" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="H101" s="7">
         <v>208</v>
       </c>
-      <c r="I101" t="s">
+      <c r="I101" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="L101">
-        <v>1044</v>
-      </c>
-      <c r="M101" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="L101" s="7">
+        <v>1056</v>
+      </c>
+      <c r="M101" s="7" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A102" s="7">
-        <v>629735</v>
+        <v>629759</v>
       </c>
       <c r="B102" s="7">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D102">
+        <v>352</v>
+      </c>
+      <c r="D102" s="7">
         <v>102</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="F102">
-        <v>20</v>
-      </c>
-      <c r="G102" t="s">
-        <v>246</v>
-      </c>
-      <c r="H102">
+      <c r="F102" s="7">
+        <v>18</v>
+      </c>
+      <c r="G102" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="H102" s="7">
         <v>208</v>
       </c>
-      <c r="I102" t="s">
+      <c r="I102" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="J102" t="s">
-        <v>340</v>
-      </c>
-      <c r="K102" t="s">
-        <v>316</v>
-      </c>
-      <c r="L102">
-        <v>1041</v>
-      </c>
-      <c r="M102" t="s">
-        <v>312</v>
-      </c>
-      <c r="N102">
-        <v>1042</v>
-      </c>
-      <c r="O102" t="s">
-        <v>313</v>
-      </c>
-      <c r="P102">
-        <v>1051</v>
-      </c>
-      <c r="Q102" t="s">
-        <v>315</v>
-      </c>
-      <c r="R102">
-        <v>1052</v>
-      </c>
-      <c r="S102" t="s">
-        <v>341</v>
-      </c>
-      <c r="T102">
-        <v>1043</v>
-      </c>
-      <c r="U102" t="s">
-        <v>314</v>
-      </c>
-      <c r="V102">
-        <v>1046</v>
-      </c>
-      <c r="W102" t="s">
-        <v>317</v>
+      <c r="L102" s="7">
+        <v>1057</v>
+      </c>
+      <c r="M102" s="7" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="103" spans="1:23" x14ac:dyDescent="0.45">
@@ -5627,10 +5615,10 @@
         <v>249</v>
       </c>
       <c r="F103">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G103" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H103">
         <v>208</v>
@@ -5638,196 +5626,445 @@
       <c r="I103" t="s">
         <v>268</v>
       </c>
+      <c r="J103" t="s">
+        <v>339</v>
+      </c>
       <c r="L103">
-        <v>1046</v>
+        <v>1041</v>
       </c>
       <c r="M103" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="104" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A104">
-        <v>629758</v>
+        <v>629747</v>
       </c>
       <c r="B104">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C104" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D104">
-        <v>95073</v>
+        <v>102</v>
       </c>
       <c r="E104" t="s">
-        <v>129</v>
+        <v>249</v>
       </c>
       <c r="F104">
-        <v>279357</v>
+        <v>19</v>
       </c>
       <c r="G104" t="s">
-        <v>116</v>
+        <v>245</v>
       </c>
       <c r="H104">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I104" t="s">
-        <v>269</v>
-      </c>
-      <c r="J104" s="3" t="s">
-        <v>342</v>
+        <v>268</v>
       </c>
       <c r="L104">
-        <v>1047</v>
+        <v>1042</v>
       </c>
       <c r="M104" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="105" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A105">
+        <v>629747</v>
+      </c>
+      <c r="B105">
+        <v>26</v>
+      </c>
+      <c r="C105" t="s">
+        <v>155</v>
+      </c>
+      <c r="D105">
+        <v>102</v>
+      </c>
+      <c r="E105" t="s">
+        <v>249</v>
+      </c>
+      <c r="F105">
+        <v>19</v>
+      </c>
+      <c r="G105" t="s">
+        <v>245</v>
+      </c>
+      <c r="H105">
+        <v>208</v>
+      </c>
+      <c r="I105" t="s">
+        <v>268</v>
+      </c>
+      <c r="L105">
+        <v>1043</v>
+      </c>
+      <c r="M105" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="106" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A106">
+        <v>629747</v>
+      </c>
+      <c r="B106">
+        <v>26</v>
+      </c>
+      <c r="C106" t="s">
+        <v>155</v>
+      </c>
+      <c r="D106">
+        <v>102</v>
+      </c>
+      <c r="E106" t="s">
+        <v>249</v>
+      </c>
+      <c r="F106">
+        <v>19</v>
+      </c>
+      <c r="G106" t="s">
+        <v>245</v>
+      </c>
+      <c r="H106">
+        <v>208</v>
+      </c>
+      <c r="I106" t="s">
+        <v>268</v>
+      </c>
+      <c r="L106">
+        <v>1044</v>
+      </c>
+      <c r="M106" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="107" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A107" s="7">
+        <v>629756</v>
+      </c>
+      <c r="B107" s="7">
+        <v>15</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="D107" s="7">
+        <v>102</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F107" s="7">
+        <v>19</v>
+      </c>
+      <c r="G107" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="H107" s="7">
+        <v>208</v>
+      </c>
+      <c r="I107" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="L107" s="7">
+        <v>1052</v>
+      </c>
+      <c r="M107" s="7" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A108" s="7">
+        <v>629735</v>
+      </c>
+      <c r="B108" s="7">
+        <v>22</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D108">
+        <v>102</v>
+      </c>
+      <c r="E108" t="s">
+        <v>249</v>
+      </c>
+      <c r="F108">
+        <v>20</v>
+      </c>
+      <c r="G108" t="s">
+        <v>246</v>
+      </c>
+      <c r="H108">
+        <v>208</v>
+      </c>
+      <c r="I108" t="s">
+        <v>268</v>
+      </c>
+      <c r="J108" t="s">
+        <v>340</v>
+      </c>
+      <c r="K108" t="s">
+        <v>316</v>
+      </c>
+      <c r="L108">
+        <v>1041</v>
+      </c>
+      <c r="M108" t="s">
+        <v>312</v>
+      </c>
+      <c r="N108">
+        <v>1042</v>
+      </c>
+      <c r="O108" t="s">
+        <v>313</v>
+      </c>
+      <c r="P108">
+        <v>1051</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>315</v>
+      </c>
+      <c r="R108">
+        <v>1052</v>
+      </c>
+      <c r="S108" t="s">
+        <v>341</v>
+      </c>
+      <c r="T108">
+        <v>1043</v>
+      </c>
+      <c r="U108" t="s">
+        <v>314</v>
+      </c>
+      <c r="V108">
+        <v>1046</v>
+      </c>
+      <c r="W108" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A109">
+        <v>629747</v>
+      </c>
+      <c r="B109">
+        <v>26</v>
+      </c>
+      <c r="C109" t="s">
+        <v>155</v>
+      </c>
+      <c r="D109">
+        <v>102</v>
+      </c>
+      <c r="E109" t="s">
+        <v>249</v>
+      </c>
+      <c r="F109">
+        <v>20</v>
+      </c>
+      <c r="G109" t="s">
+        <v>246</v>
+      </c>
+      <c r="H109">
+        <v>208</v>
+      </c>
+      <c r="I109" t="s">
+        <v>268</v>
+      </c>
+      <c r="L109">
+        <v>1046</v>
+      </c>
+      <c r="M109" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="110" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A110">
         <v>629748</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B110" t="s">
         <v>156</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C110" t="s">
         <v>157</v>
       </c>
-      <c r="D105">
+      <c r="D110">
         <v>95073</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E110" t="s">
         <v>129</v>
       </c>
-      <c r="F105">
+      <c r="F110">
         <v>279357</v>
       </c>
-      <c r="G105" t="s">
+      <c r="G110" t="s">
         <v>116</v>
       </c>
-      <c r="H105">
+      <c r="H110">
         <v>1198</v>
       </c>
-      <c r="I105" t="s">
+      <c r="I110" t="s">
         <v>48</v>
       </c>
-      <c r="L105">
+      <c r="L110">
         <v>1048</v>
       </c>
-      <c r="M105" t="s">
+      <c r="M110" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A106" s="6">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A111">
+        <v>629758</v>
+      </c>
+      <c r="B111">
+        <v>17</v>
+      </c>
+      <c r="C111" t="s">
+        <v>163</v>
+      </c>
+      <c r="D111">
+        <v>95073</v>
+      </c>
+      <c r="E111" t="s">
+        <v>129</v>
+      </c>
+      <c r="F111">
+        <v>279357</v>
+      </c>
+      <c r="G111" t="s">
+        <v>116</v>
+      </c>
+      <c r="H111">
+        <v>209</v>
+      </c>
+      <c r="I111" t="s">
+        <v>269</v>
+      </c>
+      <c r="J111" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="L111">
+        <v>1047</v>
+      </c>
+      <c r="M111" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="112" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A112" s="6">
         <v>629754</v>
       </c>
-      <c r="B106" s="6">
+      <c r="B112" s="6">
         <v>13</v>
       </c>
-      <c r="C106" s="6" t="s">
+      <c r="C112" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D106" s="6">
+      <c r="D112" s="6">
         <v>53869</v>
       </c>
-      <c r="E106" s="6" t="s">
+      <c r="E112" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="F106" s="6">
+      <c r="F112" s="6">
         <v>265065</v>
       </c>
-      <c r="G106" s="6" t="s">
+      <c r="G112" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H106" s="6">
+      <c r="H112" s="6">
         <v>772</v>
       </c>
-      <c r="I106" s="6" t="s">
+      <c r="I112" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="J106" s="6"/>
-      <c r="L106" s="6">
+      <c r="J112" s="6"/>
+      <c r="L112" s="6">
         <v>112424</v>
       </c>
-      <c r="M106" s="6" t="s">
+      <c r="M112" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="N106" s="6"/>
-    </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A107" s="6">
+      <c r="N112" s="6"/>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A113" s="6">
         <v>629754</v>
       </c>
-      <c r="B107" s="6">
+      <c r="B113" s="6">
         <v>13</v>
       </c>
-      <c r="C107" s="6" t="s">
+      <c r="C113" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D107" s="6">
+      <c r="D113" s="6">
         <v>53869</v>
       </c>
-      <c r="E107" s="6" t="s">
+      <c r="E113" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="F107" s="6">
+      <c r="F113" s="6">
         <v>265065</v>
       </c>
-      <c r="G107" s="6" t="s">
+      <c r="G113" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H107" s="6">
+      <c r="H113" s="6">
         <v>772</v>
       </c>
-      <c r="I107" s="6" t="s">
+      <c r="I113" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="J107" s="6"/>
-      <c r="L107" s="6">
+      <c r="J113" s="6"/>
+      <c r="L113" s="6">
         <v>95591</v>
       </c>
-      <c r="M107" s="6" t="s">
+      <c r="M113" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="N107" s="6"/>
-    </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A108" s="8">
+      <c r="N113" s="6"/>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A114" s="8">
         <v>629757</v>
       </c>
-      <c r="B108" s="8">
+      <c r="B114" s="8">
         <v>16</v>
       </c>
-      <c r="C108" s="8" t="s">
+      <c r="C114" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="D108" s="8">
+      <c r="D114" s="8">
         <v>18663</v>
       </c>
-      <c r="E108" s="8" t="s">
+      <c r="E114" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="F108" s="8">
+      <c r="F114" s="8">
         <v>312178</v>
       </c>
-      <c r="G108" s="8" t="s">
+      <c r="G114" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="H108" s="8">
+      <c r="H114" s="8">
         <v>594</v>
       </c>
-      <c r="I108" s="8" t="s">
+      <c r="I114" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="J108" s="8"/>
-      <c r="L108" s="8">
+      <c r="J114" s="8"/>
+      <c r="L114" s="8">
         <v>130283</v>
       </c>
-      <c r="M108" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="N108" s="8"/>
+      <c r="M114" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="N114" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5839,7 +6076,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+      <selection activeCell="A26" sqref="A26:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6160,7 +6397,7 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
@@ -6171,7 +6408,7 @@
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
@@ -6182,7 +6419,7 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -6193,7 +6430,7 @@
         <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D24">
         <v>1090</v>
@@ -6207,7 +6444,7 @@
         <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -6218,7 +6455,7 @@
         <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D26">
         <v>1088</v>
@@ -6235,7 +6472,7 @@
         <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D27">
         <v>1087</v>
@@ -6252,7 +6489,7 @@
         <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D28">
         <v>1089</v>
@@ -6269,7 +6506,10 @@
         <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>353</v>
+        <v>352</v>
+      </c>
+      <c r="E29" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -7086,7 +7326,7 @@
         <v>1039</v>
       </c>
       <c r="B9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C9" t="s">
         <v>207</v>
@@ -7264,10 +7504,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D5152B9-B788-4BDE-A1B2-C618945E4F4F}">
-  <dimension ref="A1:B133"/>
+  <dimension ref="A1:B139"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83:B83"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="B132" sqref="A132:B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8337,8 +8577,51 @@
         <v>130283</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>344</v>
-      </c>
+        <v>343</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A134">
+        <v>1053</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A135">
+        <v>1054</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A136" s="7">
+        <v>1055</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A137" s="7">
+        <v>1056</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A138" s="7">
+        <v>1057</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B139" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>